<commit_message>
B-B and C-C table update
</commit_message>
<xml_diff>
--- a/Human DM Topics.xlsx
+++ b/Human DM Topics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raquel\Desktop\Decision Making App\dec-making-app-v31.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raquel\Desktop\Decision Making App\dec-making-app-v32.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4A5C38-8CED-429C-ABE6-5E6833C0E026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CAEB12-13ED-4792-892A-82128794DA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-3915" windowWidth="17910" windowHeight="12450" xr2:uid="{3F1DC614-74A3-41B9-8627-AC851E07792B}"/>
+    <workbookView xWindow="2835" yWindow="1905" windowWidth="17910" windowHeight="12450" xr2:uid="{3F1DC614-74A3-41B9-8627-AC851E07792B}"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="243">
   <si>
     <t>Approach-Avoid Tasks</t>
   </si>
@@ -484,9 +484,6 @@
     <t>Benefit-Benefit</t>
   </si>
   <si>
-    <t>1,2</t>
-  </si>
-  <si>
     <t>23) Christmas Party</t>
   </si>
   <si>
@@ -526,8 +523,24 @@
     <t>14,20,21</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">5,16, </t>
+    <t>4,11,13</t>
+  </si>
+  <si>
+    <t>17)Health</t>
+  </si>
+  <si>
+    <t>2,5,6</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1,7,12</t>
     </r>
     <r>
       <rPr>
@@ -538,28 +551,29 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>24</t>
-    </r>
-  </si>
-  <si>
-    <t>4,11,13</t>
-  </si>
-  <si>
-    <t>17)Health</t>
-  </si>
-  <si>
-    <t>2,5,6</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1,7,12</t>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>20</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>8, 23</t>
     </r>
     <r>
       <rPr>
@@ -580,19 +594,19 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>20</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>8, 23</t>
+      <t xml:space="preserve"> 27</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3, 24</t>
     </r>
     <r>
       <rPr>
@@ -613,19 +627,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 27</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>15,</t>
+      <t xml:space="preserve"> 25</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>10, 14</t>
     </r>
     <r>
       <rPr>
@@ -636,19 +643,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 28,29</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3, 24</t>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 26</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>11, 16</t>
     </r>
     <r>
       <rPr>
@@ -659,6 +669,104 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>,17,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>18</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,19,21,22</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">18) Party games </t>
+  </si>
+  <si>
+    <t>18)Health</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 24,25</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 28,29</t>
+    </r>
+  </si>
+  <si>
+    <t>19)Party games</t>
+  </si>
+  <si>
+    <t>19)Party</t>
+  </si>
+  <si>
+    <t>19)Trip</t>
+  </si>
+  <si>
+    <r>
+      <t>12, 21</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>,</t>
     </r>
     <r>
@@ -669,12 +777,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 25</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10, 14</t>
+      <t>22</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2, 17</t>
     </r>
     <r>
       <rPr>
@@ -695,12 +803,28 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 26</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>11, 16</t>
+      <t>18</t>
+    </r>
+  </si>
+  <si>
+    <t>4,9,14</t>
+  </si>
+  <si>
+    <t>3,7, 20</t>
+  </si>
+  <si>
+    <t>5, 13, 19</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
     </r>
     <r>
       <rPr>
@@ -711,7 +835,181 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>,17,</t>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>11</t>
+    </r>
+  </si>
+  <si>
+    <t>1, 15, 16</t>
+  </si>
+  <si>
+    <t>20) Trip accomodation</t>
+  </si>
+  <si>
+    <t>20)Food</t>
+  </si>
+  <si>
+    <t>20) Entertainment</t>
+  </si>
+  <si>
+    <t>21) Trip adventures</t>
+  </si>
+  <si>
+    <t>21) Entertainment</t>
+  </si>
+  <si>
+    <t>21)Transportation</t>
+  </si>
+  <si>
+    <t>22)Transportation</t>
+  </si>
+  <si>
+    <t>22) Trip</t>
+  </si>
+  <si>
+    <t>23)Travel destinations</t>
+  </si>
+  <si>
+    <t>23) Transportation</t>
+  </si>
+  <si>
+    <t>23)Food</t>
+  </si>
+  <si>
+    <t>24)</t>
+  </si>
+  <si>
+    <t>24) Park with excuisite flowers and plants</t>
+  </si>
+  <si>
+    <t>24) Flu</t>
+  </si>
+  <si>
+    <t>24)Transportation</t>
+  </si>
+  <si>
+    <t>24)Food</t>
+  </si>
+  <si>
+    <t>25) Trip to foreign country</t>
+  </si>
+  <si>
+    <t>25) Nausea</t>
+  </si>
+  <si>
+    <t>26) Restaurent</t>
+  </si>
+  <si>
+    <t>26) Late night craving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27) Party </t>
+  </si>
+  <si>
+    <t>27) Movie night</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28) Movie </t>
+  </si>
+  <si>
+    <t>28)Entertainment</t>
+  </si>
+  <si>
+    <t>29) Concert</t>
+  </si>
+  <si>
+    <t>29) Entertainment</t>
+  </si>
+  <si>
+    <t>5,16, 24</t>
+  </si>
+  <si>
+    <t>15, 28,29</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 22,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>23</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>17,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -732,16 +1030,413 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>,19,21,22</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">18) Party games </t>
-  </si>
-  <si>
-    <t>18)Health</t>
-  </si>
-  <si>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 19</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>20,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">21 </t>
+    </r>
+  </si>
+  <si>
+    <t>1,2,6,7,10,16</t>
+  </si>
+  <si>
+    <r>
+      <t>11,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 26, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>27</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>12</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>13</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>14</t>
+    </r>
+  </si>
+  <si>
+    <t>8, 23,24</t>
+  </si>
+  <si>
+    <t>14, 23,24</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4, 8</t>
+    </r>
+  </si>
+  <si>
+    <t>6, 18, 19</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2, 13</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>21</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7,15,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 22</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>16</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>17</t>
+    </r>
+  </si>
+  <si>
+    <t>3,9, 20</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>11,12</t>
+    </r>
+  </si>
+  <si>
+    <t>1, 11, 13</t>
+  </si>
+  <si>
+    <t>5, 12,19</t>
+  </si>
+  <si>
+    <t>6, 10, 22</t>
+  </si>
+  <si>
+    <t>2, 14, 15</t>
+  </si>
+  <si>
+    <t>8, 17, 18</t>
+  </si>
+  <si>
+    <t>9, 20, 21</t>
+  </si>
+  <si>
+    <t>3,7, 16</t>
+  </si>
+  <si>
+    <t>4, 23, 24</t>
+  </si>
+  <si>
+    <t>8, 22, 23</t>
+  </si>
+  <si>
+    <t>10, 16, 17</t>
+  </si>
+  <si>
+    <t>12, 18, 24</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -761,52 +1456,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, 22,23</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, 24,25</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>17</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">, </t>
     </r>
     <r>
@@ -817,645 +1466,20 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>18</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, 19</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>15</t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, 28,29</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">8, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">20,21 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1,2,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>6,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>7,10</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,16</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>11,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 26, 27</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,12,13,14</t>
-    </r>
-  </si>
-  <si>
-    <t>19)Party games</t>
-  </si>
-  <si>
-    <t>19)Party</t>
-  </si>
-  <si>
-    <t>19)Trip</t>
-  </si>
-  <si>
-    <r>
-      <t>12, 21</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>22</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>2, 17</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>18</t>
-    </r>
-  </si>
-  <si>
-    <t>4,9,14</t>
-  </si>
-  <si>
-    <t>3,7, 20</t>
-  </si>
-  <si>
-    <t>5, 13, 19</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>6</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>11</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">8, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>23,24</t>
-    </r>
-  </si>
-  <si>
-    <t>1, 15, 16</t>
-  </si>
-  <si>
-    <t>20) Trip accomodation</t>
-  </si>
-  <si>
-    <t>20)Food</t>
-  </si>
-  <si>
-    <t>20) Entertainment</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">14, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>23,24</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, 8</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>6,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 18, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>19</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>2,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 13</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, 21</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>7,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>15,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 22</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,16,17</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>3,</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>20</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,11,12</t>
-    </r>
-  </si>
-  <si>
-    <t>21) Trip adventures</t>
-  </si>
-  <si>
-    <t>21) Entertainment</t>
-  </si>
-  <si>
-    <t>21)Transportation</t>
-  </si>
-  <si>
-    <t>1, 11</t>
-  </si>
-  <si>
-    <t>5, 12</t>
-  </si>
-  <si>
-    <t>6, 10</t>
-  </si>
-  <si>
-    <t>3,7</t>
-  </si>
-  <si>
-    <t>22)Transportation</t>
-  </si>
-  <si>
-    <t>22) Trip</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>9</t>
-    </r>
-  </si>
-  <si>
-    <t>4,11</t>
-  </si>
-  <si>
-    <t>6,7</t>
-  </si>
-  <si>
-    <t>23)Travel destinations</t>
-  </si>
-  <si>
-    <t>23) Transportation</t>
-  </si>
-  <si>
-    <t>23)Food</t>
-  </si>
-  <si>
-    <t>24)</t>
-  </si>
-  <si>
-    <t>24) Park with excuisite flowers and plants</t>
-  </si>
-  <si>
-    <t>24) Flu</t>
-  </si>
-  <si>
-    <t>24)Transportation</t>
-  </si>
-  <si>
-    <t>24)Food</t>
-  </si>
-  <si>
-    <t>25) Trip to foreign country</t>
-  </si>
-  <si>
-    <t>25) Nausea</t>
-  </si>
-  <si>
-    <t>26) Restaurent</t>
-  </si>
-  <si>
-    <t>26) Late night craving</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27) Party </t>
-  </si>
-  <si>
-    <t>27) Movie night</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28) Movie </t>
-  </si>
-  <si>
-    <t>28)Entertainment</t>
-  </si>
-  <si>
-    <t>29) Concert</t>
-  </si>
-  <si>
-    <t>29) Entertainment</t>
+  </si>
+  <si>
+    <t>4,11, 14</t>
+  </si>
+  <si>
+    <t>6,7, 21</t>
+  </si>
+  <si>
+    <t>3, 19, 20</t>
+  </si>
+  <si>
+    <t>1,2, 13</t>
   </si>
 </sst>
 </file>
@@ -1581,7 +1605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1595,8 +1619,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1914,7 +1939,7 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="J17" sqref="J17:Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1960,7 +1985,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -1989,7 +2014,7 @@
         <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -2214,7 +2239,7 @@
         <v>82</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>83</v>
@@ -2237,7 +2262,7 @@
         <v>88</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>89</v>
@@ -2260,7 +2285,7 @@
         <v>94</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>95</v>
@@ -2361,34 +2386,34 @@
         <v>124</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I17" t="s">
         <v>125</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="K17" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="M17" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="L17" t="s">
-        <v>126</v>
-      </c>
-      <c r="M17" t="s">
+      <c r="N17" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q17" s="14" t="s">
         <v>162</v>
-      </c>
-      <c r="P17" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -2405,34 +2430,34 @@
         <v>130</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I18" t="s">
         <v>131</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="L18" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="K18" s="13" t="s">
+      <c r="M18" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="N18" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="L18" s="13" t="s">
+      <c r="O18" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="P18" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="M18" s="13" t="s">
+      <c r="Q18" s="14" t="s">
         <v>169</v>
-      </c>
-      <c r="N18" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="O18" t="s">
-        <v>132</v>
-      </c>
-      <c r="P18" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -2443,40 +2468,40 @@
         <v>134</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="I19" t="s">
         <v>136</v>
       </c>
-      <c r="J19" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="K19" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="L19" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="M19" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="N19" t="s">
-        <v>179</v>
-      </c>
-      <c r="O19" t="s">
-        <v>180</v>
-      </c>
-      <c r="P19" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q19" s="13" t="s">
-        <v>182</v>
+      <c r="J19" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="L19" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="M19" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="N19" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="O19" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="P19" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q19" s="15" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -2487,40 +2512,40 @@
         <v>138</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="I20" t="s">
         <v>139</v>
       </c>
-      <c r="J20" t="s">
-        <v>186</v>
-      </c>
-      <c r="K20" t="s">
-        <v>187</v>
-      </c>
-      <c r="L20" t="s">
-        <v>188</v>
-      </c>
-      <c r="M20" t="s">
-        <v>189</v>
-      </c>
-      <c r="N20" t="s">
-        <v>190</v>
-      </c>
-      <c r="O20" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="P20" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>193</v>
+      <c r="J20" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>178</v>
+      </c>
+      <c r="L20" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="M20" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="N20" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="O20" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="P20" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q20" s="14" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -2531,40 +2556,40 @@
         <v>141</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="I21" t="s">
         <v>142</v>
       </c>
-      <c r="J21" t="s">
-        <v>197</v>
-      </c>
-      <c r="K21" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="L21" t="s">
-        <v>199</v>
-      </c>
-      <c r="M21" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="N21" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="O21" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="P21" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q21" s="13" t="s">
-        <v>204</v>
+      <c r="J21" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="L21" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="N21" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="O21" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="P21" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q21" s="15" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -2575,40 +2600,40 @@
         <v>144</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="I22" t="s">
         <v>145</v>
       </c>
-      <c r="J22" t="s">
-        <v>208</v>
-      </c>
-      <c r="K22" t="s">
-        <v>209</v>
-      </c>
-      <c r="L22" t="s">
-        <v>210</v>
-      </c>
-      <c r="M22">
-        <v>2</v>
-      </c>
-      <c r="N22">
-        <v>8</v>
-      </c>
-      <c r="O22">
-        <v>9</v>
-      </c>
-      <c r="P22" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q22">
-        <v>4</v>
+      <c r="J22" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="L22" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="M22" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="N22" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="O22" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="P22" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q22" s="14" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -2619,114 +2644,114 @@
         <v>147</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="I23" t="s">
         <v>148</v>
       </c>
-      <c r="J23">
-        <v>8</v>
-      </c>
-      <c r="K23">
-        <v>10</v>
-      </c>
-      <c r="L23">
-        <v>12</v>
-      </c>
-      <c r="M23" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="N23" t="s">
-        <v>215</v>
-      </c>
-      <c r="O23" t="s">
-        <v>216</v>
-      </c>
-      <c r="P23">
-        <v>3</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>149</v>
+      <c r="J23" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="L23" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="M23" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="N23" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="O23" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="P23" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q23" s="14" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>151</v>
-      </c>
       <c r="C24" s="6" t="s">
-        <v>217</v>
+        <v>192</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>219</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>220</v>
+        <v>195</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>222</v>
+        <v>196</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>197</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>226</v>
+        <v>200</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
-        <v>227</v>
+        <v>202</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>228</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B28" s="9" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
-        <v>231</v>
+        <v>206</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2976,35 +3001,35 @@
       </c>
       <c r="B7" t="str">
         <f>Topics!J22</f>
-        <v>1, 11</v>
+        <v>1, 11, 13</v>
       </c>
       <c r="C7" t="str">
         <f>Topics!K22</f>
-        <v>5, 12</v>
+        <v>5, 12,19</v>
       </c>
       <c r="D7" t="str">
         <f>Topics!L22</f>
-        <v>6, 10</v>
-      </c>
-      <c r="E7">
+        <v>6, 10, 22</v>
+      </c>
+      <c r="E7" t="str">
         <f>Topics!M22</f>
-        <v>2</v>
-      </c>
-      <c r="F7">
+        <v>2, 14, 15</v>
+      </c>
+      <c r="F7" t="str">
         <f>Topics!N22</f>
-        <v>8</v>
-      </c>
-      <c r="G7">
+        <v>8, 17, 18</v>
+      </c>
+      <c r="G7" t="str">
         <f>Topics!O22</f>
-        <v>9</v>
+        <v>9, 20, 21</v>
       </c>
       <c r="H7" t="str">
         <f>Topics!P22</f>
-        <v>3,7</v>
-      </c>
-      <c r="I7">
+        <v>3,7, 16</v>
+      </c>
+      <c r="I7" t="str">
         <f>Topics!Q22</f>
-        <v>4</v>
+        <v>4, 23, 24</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3012,37 +3037,37 @@
         <f>Topics!I23</f>
         <v>Benefit-Benefit</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="str">
         <f>Topics!J23</f>
-        <v>8</v>
-      </c>
-      <c r="C8">
+        <v>8, 22, 23</v>
+      </c>
+      <c r="C8" t="str">
         <f>Topics!K23</f>
-        <v>10</v>
-      </c>
-      <c r="D8">
+        <v>10, 16, 17</v>
+      </c>
+      <c r="D8" t="str">
         <f>Topics!L23</f>
-        <v>12</v>
+        <v>12, 18, 24</v>
       </c>
       <c r="E8" t="str">
         <f>Topics!M23</f>
-        <v>5,9</v>
+        <v>5,9, 15</v>
       </c>
       <c r="F8" t="str">
         <f>Topics!N23</f>
-        <v>4,11</v>
+        <v>4,11, 14</v>
       </c>
       <c r="G8" t="str">
         <f>Topics!O23</f>
-        <v>6,7</v>
-      </c>
-      <c r="H8">
+        <v>6,7, 21</v>
+      </c>
+      <c r="H8" t="str">
         <f>Topics!P23</f>
-        <v>3</v>
+        <v>3, 19, 20</v>
       </c>
       <c r="I8" t="str">
         <f>Topics!Q23</f>
-        <v>1,2</v>
+        <v>1,2, 13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>